<commit_message>
Fixes, Began adding chart support
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="XLLinked" sheetId="1" r:id="rId1"/>
+    <sheet name="Without" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>Mon</t>
   </si>
@@ -26,9 +27,6 @@
   </si>
   <si>
     <t>Thur</t>
-  </si>
-  <si>
-    <t>Meal</t>
   </si>
   <si>
     <t>Breakfast</t>
@@ -111,6 +109,737 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Breakfast</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'XLLinked'!B1:E1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Weds</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thur</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'XLLinked'!B2:E2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Lunch</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'XLLinked'!B1:E1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Weds</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thur</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'XLLinked'!B3:E3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Dinner</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'XLLinked'!B1:E1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Weds</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thur</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'XLLinked'!B4:E4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Midnight Snack</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'XLLinked'!B1:E1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Weds</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thur</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'XLLinked'!B5:E5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50010001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50010002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'XLLinked'!A2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Breakfast</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'XLLinked'!B1:E1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Weds</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thur</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'XLLinked'!B2:B5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50020001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50020002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Without!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Breakfast</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Without!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Weds</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thur</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Without!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Without!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lunch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Without!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Weds</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thur</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Without!$B$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Without!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dinner</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Without!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Weds</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thur</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Without!$B$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Without!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Midnight Snack</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Without!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Weds</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thur</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Without!$B$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50030001"/>
+        <c:axId val="50030002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50030001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50030002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50030002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50030001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,9 +1134,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,7 +1149,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>15</v>
@@ -440,7 +1166,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -457,7 +1183,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>12</v>
@@ -474,7 +1200,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -491,5 +1217,102 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>22</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added chart support/ basic tests
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -8,14 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="XLLinked" sheetId="1" r:id="rId1"/>
-    <sheet name="Without" sheetId="2" r:id="rId2"/>
+    <sheet name="scatter" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Mon</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t>Midnight Snack</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -115,6 +124,24 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>With xl_link</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -124,31 +151,31 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Breakfast</c:v>
+            <c:v>Mon</c:v>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'XLLinked'!B1:E1</c:f>
+              <c:f>'XLLinked'!A2:A5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Mon</c:v>
+                  <c:v>Breakfast</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tues</c:v>
+                  <c:v>Lunch</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Weds</c:v>
+                  <c:v>Dinner</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Thur</c:v>
+                  <c:v>Midnight Snack</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'XLLinked'!B2:E2</c:f>
+              <c:f>'XLLinked'!B2:B5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -156,13 +183,13 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -172,45 +199,45 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Lunch</c:v>
+            <c:v>Tues</c:v>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'XLLinked'!B1:E1</c:f>
+              <c:f>'XLLinked'!A2:A5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Mon</c:v>
+                  <c:v>Breakfast</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tues</c:v>
+                  <c:v>Lunch</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Weds</c:v>
+                  <c:v>Dinner</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Thur</c:v>
+                  <c:v>Midnight Snack</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'XLLinked'!B3:E3</c:f>
+              <c:f>'XLLinked'!C2:C5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -220,45 +247,45 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Dinner</c:v>
+            <c:v>Weds</c:v>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'XLLinked'!B1:E1</c:f>
+              <c:f>'XLLinked'!A2:A5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Mon</c:v>
+                  <c:v>Breakfast</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tues</c:v>
+                  <c:v>Lunch</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Weds</c:v>
+                  <c:v>Dinner</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Thur</c:v>
+                  <c:v>Midnight Snack</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'XLLinked'!B4:E4</c:f>
+              <c:f>'XLLinked'!D2:D5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -268,42 +295,42 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Midnight Snack</c:v>
+            <c:v>Thur</c:v>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'XLLinked'!B1:E1</c:f>
+              <c:f>'XLLinked'!A2:A5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Mon</c:v>
+                  <c:v>Breakfast</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Tues</c:v>
+                  <c:v>Lunch</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Weds</c:v>
+                  <c:v>Dinner</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Thur</c:v>
+                  <c:v>Midnight Snack</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'XLLinked'!B5:E5</c:f>
+              <c:f>'XLLinked'!E2:E5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>9</c:v>
@@ -321,6 +348,24 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Meal</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010002"/>
         <c:crosses val="autoZero"/>
@@ -335,6 +380,24 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Calories</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010001"/>
@@ -360,372 +423,271 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Scatter Example</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'XLLinked'!A2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Breakfast</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Y1</c:v>
           </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'XLLinked'!B1:E1</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Mon</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Tues</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Weds</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Thur</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
             <c:numRef>
-              <c:f>'XLLinked'!B2:B5</c:f>
+              <c:f>'scatter'!A2:A11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'scatter'!B2:B11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Y2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'scatter'!A2:A11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'scatter'!C2:C11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
         </c:ser>
         <c:axId val="50020001"/>
         <c:axId val="50020002"/>
-      </c:barChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="50020001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>x</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50020002"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="50020002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>y</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50020001"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Without!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Breakfast</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Without!$B$1:$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Mon</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Tues</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Weds</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Thur</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Without!$B$2:$E$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Without!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Lunch</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Without!$B$1:$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Mon</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Tues</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Weds</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Thur</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Without!$B$3:$E$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Without!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Dinner</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Without!$B$1:$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Mon</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Tues</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Weds</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Thur</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Without!$B$4:$E$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Without!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Midnight Snack</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Without!$B$1:$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Mon</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Tues</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Weds</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Thur</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Without!$B$5:$E$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="50030001"/>
-        <c:axId val="50030002"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="50030001"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50030002"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="50030002"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50030001"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -774,36 +736,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -811,13 +743,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -1223,92 +1155,131 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>22</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="B4">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
         <v>7</v>
       </c>
-      <c r="B5">
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
         <v>3</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="E5">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
         <v>9</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>